<commit_message>
Soil nitrogen: 1st working version
Working as in : simulation can run and not break for supposedly ever (700+ days at least) and few unexpected values.
Only NAVL (and thus SNAVL) is known to take negative values somehow. It's very likely a problem with the timestep (value to WHAT point of the timestep should we consider?) ... I will investigate.

Updated changelog, although I haven't been so rigorous on keeping notes for the past few days (a lot of small tweaks).
</commit_message>
<xml_diff>
--- a/input/managementPlans.xlsx
+++ b/input/managementPlans.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achille\Documents\GitHub\SSM.R\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F30AB6-57D3-4CD9-80E9-AEABE09FDD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9C469C0-617B-4593-A09A-72E3404908B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,17 @@
   <definedNames>
     <definedName name="Diameter">[1]Run!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -518,7 +527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E42" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="E42" authorId="0" shapeId="0" xr:uid="{5DFE0CC7-BDC1-4B53-9B95-0E1DCE5EC981}">
       <text>
         <r>
           <rPr>
@@ -570,7 +579,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E44" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="E44" authorId="0" shapeId="0" xr:uid="{0870B7BC-AD57-4F82-9FF1-50FC584AB48F}">
       <text>
         <r>
           <rPr>
@@ -2356,7 +2365,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="59">
   <si>
     <t>water = 0   for potential production</t>
   </si>
@@ -3364,8 +3373,8 @@
   <dimension ref="A1:X3956"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F182" sqref="F182"/>
+      <pane ySplit="10" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4394,7 +4403,7 @@
         <v>35</v>
       </c>
       <c r="F42" s="26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G42" s="32" t="s">
         <v>36</v>
@@ -4421,7 +4430,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="26">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -4429,7 +4438,7 @@
         <v>38</v>
       </c>
       <c r="F43" s="26">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G43" s="26">
         <v>0.25</v>
@@ -4456,7 +4465,7 @@
         <v>39</v>
       </c>
       <c r="B44" s="26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -4464,7 +4473,7 @@
         <v>39</v>
       </c>
       <c r="F44" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="30"/>
       <c r="H44" s="8"/>
@@ -4561,19 +4570,19 @@
         <v>1</v>
       </c>
       <c r="B47" s="26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C47" s="26">
+        <v>10</v>
+      </c>
+      <c r="D47" s="26">
         <v>5</v>
       </c>
-      <c r="D47" s="26">
-        <v>7</v>
-      </c>
       <c r="E47" s="26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F47" s="26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G47" s="13"/>
       <c r="H47" s="8"/>
@@ -4597,20 +4606,20 @@
       <c r="A48" s="40">
         <v>2</v>
       </c>
-      <c r="B48" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="26" t="s">
-        <v>33</v>
+      <c r="B48" s="26">
+        <v>10</v>
+      </c>
+      <c r="C48" s="26">
+        <v>10</v>
+      </c>
+      <c r="D48" s="26">
+        <v>5</v>
       </c>
       <c r="E48" s="26">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F48" s="26">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G48" s="13"/>
       <c r="H48" s="8"/>
@@ -4634,20 +4643,20 @@
       <c r="A49" s="40">
         <v>3</v>
       </c>
-      <c r="B49" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="26" t="s">
-        <v>33</v>
+      <c r="B49" s="26">
+        <v>12</v>
+      </c>
+      <c r="C49" s="26">
+        <v>10</v>
+      </c>
+      <c r="D49" s="26">
+        <v>5</v>
       </c>
       <c r="E49" s="26">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F49" s="26">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G49" s="13"/>
       <c r="H49" s="8"/>
@@ -4671,20 +4680,20 @@
       <c r="A50" s="41">
         <v>4</v>
       </c>
-      <c r="B50" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="26" t="s">
-        <v>33</v>
+      <c r="B50" s="26">
+        <v>20</v>
+      </c>
+      <c r="C50" s="26">
+        <v>10</v>
+      </c>
+      <c r="D50" s="26">
+        <v>5</v>
       </c>
       <c r="E50" s="26">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F50" s="26">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G50" s="13"/>
       <c r="H50" s="8"/>
@@ -4708,20 +4717,20 @@
       <c r="A51" s="41">
         <v>5</v>
       </c>
-      <c r="B51" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D51" s="26" t="s">
-        <v>33</v>
+      <c r="B51" s="26">
+        <v>30</v>
+      </c>
+      <c r="C51" s="26">
+        <v>10</v>
+      </c>
+      <c r="D51" s="26">
+        <v>5</v>
       </c>
       <c r="E51" s="26">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F51" s="26">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G51" s="13"/>
       <c r="H51" s="8"/>
@@ -4745,20 +4754,20 @@
       <c r="A52" s="41">
         <v>6</v>
       </c>
-      <c r="B52" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="26" t="s">
-        <v>33</v>
+      <c r="B52" s="26">
+        <v>40</v>
+      </c>
+      <c r="C52" s="26">
+        <v>10</v>
+      </c>
+      <c r="D52" s="26">
+        <v>5</v>
       </c>
       <c r="E52" s="26">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F52" s="26">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G52" s="13"/>
       <c r="H52" s="8"/>
@@ -4782,14 +4791,14 @@
       <c r="A53" s="41">
         <v>7</v>
       </c>
-      <c r="B53" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" s="26" t="s">
-        <v>33</v>
+      <c r="B53" s="26">
+        <v>0</v>
+      </c>
+      <c r="C53" s="26">
+        <v>0</v>
+      </c>
+      <c r="D53" s="26">
+        <v>0</v>
       </c>
       <c r="E53" s="26">
         <v>0</v>
@@ -4819,14 +4828,14 @@
       <c r="A54" s="41">
         <v>8</v>
       </c>
-      <c r="B54" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="26" t="s">
-        <v>33</v>
+      <c r="B54" s="26">
+        <v>0</v>
+      </c>
+      <c r="C54" s="26">
+        <v>0</v>
+      </c>
+      <c r="D54" s="26">
+        <v>0</v>
       </c>
       <c r="E54" s="26">
         <v>0</v>
@@ -4856,14 +4865,14 @@
       <c r="A55" s="41">
         <v>9</v>
       </c>
-      <c r="B55" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>33</v>
+      <c r="B55" s="26">
+        <v>0</v>
+      </c>
+      <c r="C55" s="26">
+        <v>0</v>
+      </c>
+      <c r="D55" s="26">
+        <v>0</v>
       </c>
       <c r="E55" s="26">
         <v>0</v>
@@ -4893,14 +4902,14 @@
       <c r="A56" s="42">
         <v>10</v>
       </c>
-      <c r="B56" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="C56" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="43" t="s">
-        <v>33</v>
+      <c r="B56" s="26">
+        <v>0</v>
+      </c>
+      <c r="C56" s="26">
+        <v>0</v>
+      </c>
+      <c r="D56" s="26">
+        <v>0</v>
       </c>
       <c r="E56" s="43">
         <v>0</v>
@@ -7302,7 +7311,7 @@
         <v>37</v>
       </c>
       <c r="B158" s="26">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C158" s="8"/>
       <c r="D158" s="8"/>
@@ -7325,8 +7334,8 @@
       <c r="A159" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B159" s="26" t="s">
-        <v>33</v>
+      <c r="B159" s="26">
+        <v>2</v>
       </c>
       <c r="C159" s="8"/>
       <c r="D159" s="8"/>
@@ -7397,14 +7406,14 @@
       <c r="A162" s="40">
         <v>1</v>
       </c>
-      <c r="B162" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C162" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D162" s="26" t="s">
-        <v>33</v>
+      <c r="B162" s="26">
+        <v>5</v>
+      </c>
+      <c r="C162" s="26">
+        <v>10</v>
+      </c>
+      <c r="D162" s="26">
+        <v>5</v>
       </c>
       <c r="E162" s="26">
         <v>5</v>
@@ -7423,14 +7432,14 @@
       <c r="A163" s="40">
         <v>2</v>
       </c>
-      <c r="B163" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C163" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D163" s="26" t="s">
-        <v>33</v>
+      <c r="B163" s="26">
+        <v>10</v>
+      </c>
+      <c r="C163" s="26">
+        <v>10</v>
+      </c>
+      <c r="D163" s="26">
+        <v>5</v>
       </c>
       <c r="E163" s="26">
         <v>10</v>
@@ -7449,14 +7458,14 @@
       <c r="A164" s="40">
         <v>3</v>
       </c>
-      <c r="B164" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C164" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D164" s="26" t="s">
-        <v>33</v>
+      <c r="B164" s="26">
+        <v>12</v>
+      </c>
+      <c r="C164" s="26">
+        <v>10</v>
+      </c>
+      <c r="D164" s="26">
+        <v>5</v>
       </c>
       <c r="E164" s="26">
         <v>12</v>
@@ -7475,14 +7484,14 @@
       <c r="A165" s="41">
         <v>4</v>
       </c>
-      <c r="B165" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C165" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D165" s="26" t="s">
-        <v>33</v>
+      <c r="B165" s="26">
+        <v>20</v>
+      </c>
+      <c r="C165" s="26">
+        <v>10</v>
+      </c>
+      <c r="D165" s="26">
+        <v>5</v>
       </c>
       <c r="E165" s="26">
         <v>20</v>
@@ -7501,14 +7510,14 @@
       <c r="A166" s="41">
         <v>5</v>
       </c>
-      <c r="B166" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C166" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D166" s="26" t="s">
-        <v>33</v>
+      <c r="B166" s="26">
+        <v>30</v>
+      </c>
+      <c r="C166" s="26">
+        <v>10</v>
+      </c>
+      <c r="D166" s="26">
+        <v>5</v>
       </c>
       <c r="E166" s="26">
         <v>30</v>
@@ -7527,14 +7536,14 @@
       <c r="A167" s="41">
         <v>6</v>
       </c>
-      <c r="B167" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C167" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D167" s="26" t="s">
-        <v>33</v>
+      <c r="B167" s="26">
+        <v>40</v>
+      </c>
+      <c r="C167" s="26">
+        <v>10</v>
+      </c>
+      <c r="D167" s="26">
+        <v>5</v>
       </c>
       <c r="E167" s="26">
         <v>40</v>
@@ -7553,14 +7562,14 @@
       <c r="A168" s="41">
         <v>7</v>
       </c>
-      <c r="B168" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C168" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D168" s="26" t="s">
-        <v>33</v>
+      <c r="B168" s="26">
+        <v>0</v>
+      </c>
+      <c r="C168" s="26">
+        <v>0</v>
+      </c>
+      <c r="D168" s="26">
+        <v>0</v>
       </c>
       <c r="E168" s="26">
         <v>0</v>
@@ -7579,14 +7588,14 @@
       <c r="A169" s="41">
         <v>8</v>
       </c>
-      <c r="B169" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C169" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D169" s="26" t="s">
-        <v>33</v>
+      <c r="B169" s="26">
+        <v>0</v>
+      </c>
+      <c r="C169" s="26">
+        <v>0</v>
+      </c>
+      <c r="D169" s="26">
+        <v>0</v>
       </c>
       <c r="E169" s="26">
         <v>0</v>
@@ -7605,14 +7614,14 @@
       <c r="A170" s="41">
         <v>9</v>
       </c>
-      <c r="B170" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C170" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D170" s="26" t="s">
-        <v>33</v>
+      <c r="B170" s="26">
+        <v>0</v>
+      </c>
+      <c r="C170" s="26">
+        <v>0</v>
+      </c>
+      <c r="D170" s="26">
+        <v>0</v>
       </c>
       <c r="E170" s="26">
         <v>0</v>
@@ -7631,14 +7640,14 @@
       <c r="A171" s="42">
         <v>10</v>
       </c>
-      <c r="B171" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="C171" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D171" s="43" t="s">
-        <v>33</v>
+      <c r="B171" s="26">
+        <v>0</v>
+      </c>
+      <c r="C171" s="26">
+        <v>0</v>
+      </c>
+      <c r="D171" s="26">
+        <v>0</v>
       </c>
       <c r="E171" s="43">
         <v>0</v>
@@ -7826,7 +7835,7 @@
         <v>37</v>
       </c>
       <c r="B181" s="26">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C181" s="8"/>
       <c r="D181" s="8"/>
@@ -7849,8 +7858,8 @@
       <c r="A182" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B182" s="26" t="s">
-        <v>33</v>
+      <c r="B182" s="26">
+        <v>2</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="8"/>
@@ -7921,14 +7930,14 @@
       <c r="A185" s="40">
         <v>1</v>
       </c>
-      <c r="B185" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C185" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D185" s="26" t="s">
-        <v>33</v>
+      <c r="B185" s="26">
+        <v>5</v>
+      </c>
+      <c r="C185" s="26">
+        <v>10</v>
+      </c>
+      <c r="D185" s="26">
+        <v>5</v>
       </c>
       <c r="E185" s="26">
         <v>5</v>
@@ -7947,14 +7956,14 @@
       <c r="A186" s="40">
         <v>2</v>
       </c>
-      <c r="B186" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C186" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D186" s="26" t="s">
-        <v>33</v>
+      <c r="B186" s="26">
+        <v>10</v>
+      </c>
+      <c r="C186" s="26">
+        <v>10</v>
+      </c>
+      <c r="D186" s="26">
+        <v>5</v>
       </c>
       <c r="E186" s="26">
         <v>10</v>
@@ -7973,14 +7982,14 @@
       <c r="A187" s="40">
         <v>3</v>
       </c>
-      <c r="B187" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C187" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D187" s="26" t="s">
-        <v>33</v>
+      <c r="B187" s="26">
+        <v>12</v>
+      </c>
+      <c r="C187" s="26">
+        <v>10</v>
+      </c>
+      <c r="D187" s="26">
+        <v>5</v>
       </c>
       <c r="E187" s="26">
         <v>12</v>
@@ -7999,14 +8008,14 @@
       <c r="A188" s="41">
         <v>4</v>
       </c>
-      <c r="B188" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C188" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D188" s="26" t="s">
-        <v>33</v>
+      <c r="B188" s="26">
+        <v>20</v>
+      </c>
+      <c r="C188" s="26">
+        <v>10</v>
+      </c>
+      <c r="D188" s="26">
+        <v>5</v>
       </c>
       <c r="E188" s="26">
         <v>20</v>
@@ -8025,14 +8034,14 @@
       <c r="A189" s="41">
         <v>5</v>
       </c>
-      <c r="B189" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C189" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D189" s="26" t="s">
-        <v>33</v>
+      <c r="B189" s="26">
+        <v>30</v>
+      </c>
+      <c r="C189" s="26">
+        <v>10</v>
+      </c>
+      <c r="D189" s="26">
+        <v>5</v>
       </c>
       <c r="E189" s="26">
         <v>30</v>
@@ -8051,14 +8060,14 @@
       <c r="A190" s="41">
         <v>6</v>
       </c>
-      <c r="B190" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C190" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D190" s="26" t="s">
-        <v>33</v>
+      <c r="B190" s="26">
+        <v>40</v>
+      </c>
+      <c r="C190" s="26">
+        <v>10</v>
+      </c>
+      <c r="D190" s="26">
+        <v>5</v>
       </c>
       <c r="E190" s="26">
         <v>40</v>
@@ -8077,14 +8086,14 @@
       <c r="A191" s="41">
         <v>7</v>
       </c>
-      <c r="B191" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C191" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D191" s="26" t="s">
-        <v>33</v>
+      <c r="B191" s="26">
+        <v>0</v>
+      </c>
+      <c r="C191" s="26">
+        <v>0</v>
+      </c>
+      <c r="D191" s="26">
+        <v>0</v>
       </c>
       <c r="E191" s="26">
         <v>0</v>
@@ -8103,14 +8112,14 @@
       <c r="A192" s="41">
         <v>8</v>
       </c>
-      <c r="B192" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C192" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D192" s="26" t="s">
-        <v>33</v>
+      <c r="B192" s="26">
+        <v>0</v>
+      </c>
+      <c r="C192" s="26">
+        <v>0</v>
+      </c>
+      <c r="D192" s="26">
+        <v>0</v>
       </c>
       <c r="E192" s="26">
         <v>0</v>
@@ -8129,14 +8138,14 @@
       <c r="A193" s="41">
         <v>9</v>
       </c>
-      <c r="B193" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C193" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D193" s="26" t="s">
-        <v>33</v>
+      <c r="B193" s="26">
+        <v>0</v>
+      </c>
+      <c r="C193" s="26">
+        <v>0</v>
+      </c>
+      <c r="D193" s="26">
+        <v>0</v>
       </c>
       <c r="E193" s="26">
         <v>0</v>
@@ -8155,14 +8164,14 @@
       <c r="A194" s="42">
         <v>10</v>
       </c>
-      <c r="B194" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="C194" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D194" s="43" t="s">
-        <v>33</v>
+      <c r="B194" s="26">
+        <v>0</v>
+      </c>
+      <c r="C194" s="26">
+        <v>0</v>
+      </c>
+      <c r="D194" s="26">
+        <v>0</v>
       </c>
       <c r="E194" s="43">
         <v>0</v>

</xml_diff>